<commit_message>
Bugs fix. Graphics function will add in next version.
</commit_message>
<xml_diff>
--- a/BedivereKnxClient/data.xlsx
+++ b/BedivereKnxClient/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program\Ouroboros\BedivereKnxClient\BedivereKnxClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BCAF04-C7FF-453C-A34B-2CC904712481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0105C4E6-7F34-4606-9131-0C0E8E19340C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interfaces" sheetId="4" r:id="rId1"/>
@@ -4572,30 +4572,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GrpAddr-Sw_Ctl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GrpDpt-Sw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GrpAddr-Sw_Fdb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GrpDpt-Val</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GrpAddr-Val_Ctl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GrpAddr-Val_Fdb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>InterfaceAddress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4645,6 +4621,30 @@
   </si>
   <si>
     <t>123456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sw-GrpDpt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sw-GrpAddr_Ctl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sw-GrpAddr_Fdb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Val-GrpDpt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Val-GrpAddr_Ctl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Val-GrpAddr_Fdb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5046,7 +5046,7 @@
         <v>913</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -5744,9 +5744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9671D8-C670-4FF9-9F5F-C699E4CE0AC7}">
   <dimension ref="A1:K242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5778,22 +5778,22 @@
         <v>911</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1408</v>
+        <v>1420</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1407</v>
+        <v>1421</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1409</v>
+        <v>1422</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1410</v>
+        <v>1423</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1411</v>
+        <v>1424</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>1412</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13072,7 +13072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C180A-25ED-435B-B21E-89E38876E68D}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -13086,44 +13086,44 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1414</v>
+        <v>1408</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1415</v>
+        <v>1409</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1416</v>
+        <v>1410</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1417</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1418</v>
+        <v>1412</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Table column bug fix. Add 'Enable' column to sheet 'Interface'
</commit_message>
<xml_diff>
--- a/BedivereKnxClient/data.xlsx
+++ b/BedivereKnxClient/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program\Ouroboros\BedivereKnxClient\BedivereKnxClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0105C4E6-7F34-4606-9131-0C0E8E19340C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6ACB98B-5386-4A34-97C2-2735488B106F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4624,28 +4624,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sw-GrpDpt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sw-GrpAddr_Ctl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sw-GrpAddr_Fdb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Val-GrpDpt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Val-GrpAddr_Ctl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Val-GrpAddr_Fdb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Sw_GrpDpt</t>
+  </si>
+  <si>
+    <t>Sw_Ctl_GrpAddr</t>
+  </si>
+  <si>
+    <t>Sw_Fdb_GrpAddr</t>
+  </si>
+  <si>
+    <t>Val_GrpDpt</t>
+  </si>
+  <si>
+    <t>Val_Ctl_GrpAddr</t>
+  </si>
+  <si>
+    <t>Val_Fdb_GrpAddr</t>
   </si>
 </sst>
 </file>
@@ -5746,7 +5740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5755,10 +5749,7 @@
     <col min="3" max="3" width="20.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="16.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="3" customWidth="1"/>
-    <col min="10" max="11" width="16.77734375" style="3" customWidth="1"/>
+    <col min="6" max="11" width="18.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>